<commit_message>
Case for ORH128 board
</commit_message>
<xml_diff>
--- a/pcbs/Headstages/ORH128/ORH128_Electrode_Map.xlsx
+++ b/pcbs/Headstages/ORH128/ORH128_Electrode_Map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Documents\TNEL\NACQ\pcbs\Headstages\ORH128\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="407">
   <si>
     <t>A-000</t>
   </si>
@@ -1230,14 +1230,37 @@
   </si>
   <si>
     <t>AuxSwitch: Position 1 Down (CH2) or Up (L2)</t>
+  </si>
+  <si>
+    <t>X-Pos (um)</t>
+  </si>
+  <si>
+    <t>Y-Pos (um)</t>
+  </si>
+  <si>
+    <t>Impedance</t>
+  </si>
+  <si>
+    <t>Area (mm2)</t>
+  </si>
+  <si>
+    <t>Origin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1265,8 +1288,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1286,54 +1310,240 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>8283</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>115956</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>107678</xdr:rowOff>
+      <xdr:rowOff>24848</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>144751</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>27396</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>252424</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>135066</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Group 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B609CEDD-A1BB-4C92-A6FA-3761F69C9ACA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9B03342-0102-450E-9A85-30D02DCFB7BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="2489626" y="1494313"/>
-          <a:ext cx="6206218" cy="3813947"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7263847" y="215348"/>
+          <a:ext cx="3813947" cy="6206218"/>
+          <a:chOff x="4189026" y="325891"/>
+          <a:chExt cx="3813947" cy="6206218"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="Picture 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B609CEDD-A1BB-4C92-A6FA-3761F69C9ACA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="2992891" y="1522026"/>
+            <a:ext cx="6206218" cy="3813947"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="TextBox 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F878D81F-B4B4-4E58-A09C-D49918500E31}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4816551" y="3902149"/>
+            <a:ext cx="1467293" cy="261610"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="en-US"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Origin</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B029DC03-C533-4A58-8550-4548158E1068}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5305647" y="4043587"/>
+            <a:ext cx="191385" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="3">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1636,51 +1846,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D133"/>
+  <dimension ref="A1:H133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>158</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>3.14*0.025*0.025</f>
+        <v>1.9625000000000003E-3</v>
+      </c>
+      <c r="H2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>159</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">3.14*0.025*0.025</f>
+        <v>1.9625000000000003E-3</v>
+      </c>
+      <c r="H3" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1690,11 +1931,22 @@
       <c r="C4" t="s">
         <v>162</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>50*63</f>
+        <v>3150</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+      <c r="H4" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1704,11 +1956,22 @@
       <c r="C5" t="s">
         <v>163</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>E4-50</f>
+        <v>3100</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+      <c r="H5" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1718,8 +1981,19 @@
       <c r="C6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>E5-50</f>
+        <v>3050</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1729,8 +2003,19 @@
       <c r="C7" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E67" si="1">E6-50</f>
+        <v>3000</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1740,8 +2025,19 @@
       <c r="C8" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>2950</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1751,8 +2047,19 @@
       <c r="C9" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>2900</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1762,8 +2069,19 @@
       <c r="C10" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>2850</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1773,8 +2091,19 @@
       <c r="C11" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>2800</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1784,8 +2113,19 @@
       <c r="C12" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>2750</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1795,8 +2135,19 @@
       <c r="C13" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>2700</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1806,8 +2157,19 @@
       <c r="C14" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>2650</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1817,8 +2179,19 @@
       <c r="C15" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1828,8 +2201,19 @@
       <c r="C16" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>2550</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1839,8 +2223,19 @@
       <c r="C17" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1850,8 +2245,19 @@
       <c r="C18" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>2450</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1861,8 +2267,19 @@
       <c r="C19" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>2400</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1872,8 +2289,19 @@
       <c r="C20" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>2350</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1883,8 +2311,19 @@
       <c r="C21" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>2300</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1894,8 +2333,19 @@
       <c r="C22" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>2250</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1905,8 +2355,19 @@
       <c r="C23" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1916,8 +2377,19 @@
       <c r="C24" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>2150</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1927,8 +2399,19 @@
       <c r="C25" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1938,8 +2421,19 @@
       <c r="C26" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>2050</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>295</v>
       </c>
@@ -1949,8 +2443,19 @@
       <c r="C27" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>296</v>
       </c>
@@ -1960,8 +2465,19 @@
       <c r="C28" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>1950</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>297</v>
       </c>
@@ -1971,8 +2487,19 @@
       <c r="C29" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>1900</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>298</v>
       </c>
@@ -1982,8 +2509,19 @@
       <c r="C30" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>1850</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>299</v>
       </c>
@@ -1993,8 +2531,19 @@
       <c r="C31" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>300</v>
       </c>
@@ -2004,8 +2553,19 @@
       <c r="C32" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>1750</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>301</v>
       </c>
@@ -2015,8 +2575,19 @@
       <c r="C33" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>1700</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>302</v>
       </c>
@@ -2026,8 +2597,19 @@
       <c r="C34" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>1650</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>303</v>
       </c>
@@ -2037,8 +2619,19 @@
       <c r="C35" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>1600</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>304</v>
       </c>
@@ -2048,8 +2641,19 @@
       <c r="C36" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>1550</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>305</v>
       </c>
@@ -2059,8 +2663,19 @@
       <c r="C37" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>1500</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>306</v>
       </c>
@@ -2070,8 +2685,19 @@
       <c r="C38" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>1450</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>307</v>
       </c>
@@ -2081,8 +2707,19 @@
       <c r="C39" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>1400</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>308</v>
       </c>
@@ -2092,8 +2729,19 @@
       <c r="C40" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>1350</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>309</v>
       </c>
@@ -2103,8 +2751,19 @@
       <c r="C41" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>1300</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>310</v>
       </c>
@@ -2114,8 +2773,19 @@
       <c r="C42" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>1250</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>311</v>
       </c>
@@ -2125,8 +2795,19 @@
       <c r="C43" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>312</v>
       </c>
@@ -2136,8 +2817,19 @@
       <c r="C44" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>1150</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>313</v>
       </c>
@@ -2147,8 +2839,19 @@
       <c r="C45" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>1100</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>314</v>
       </c>
@@ -2158,8 +2861,19 @@
       <c r="C46" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>1050</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>315</v>
       </c>
@@ -2169,8 +2883,19 @@
       <c r="C47" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>316</v>
       </c>
@@ -2180,8 +2905,19 @@
       <c r="C48" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>950</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>317</v>
       </c>
@@ -2191,8 +2927,19 @@
       <c r="C49" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>318</v>
       </c>
@@ -2202,8 +2949,19 @@
       <c r="C50" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>850</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>319</v>
       </c>
@@ -2213,8 +2971,19 @@
       <c r="C51" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>320</v>
       </c>
@@ -2224,8 +2993,19 @@
       <c r="C52" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>750</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>321</v>
       </c>
@@ -2235,8 +3015,19 @@
       <c r="C53" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>700</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>322</v>
       </c>
@@ -2246,8 +3037,19 @@
       <c r="C54" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="1"/>
+        <v>650</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>323</v>
       </c>
@@ -2257,8 +3059,19 @@
       <c r="C55" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>324</v>
       </c>
@@ -2268,8 +3081,19 @@
       <c r="C56" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="1"/>
+        <v>550</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>325</v>
       </c>
@@ -2279,8 +3103,19 @@
       <c r="C57" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>326</v>
       </c>
@@ -2290,8 +3125,19 @@
       <c r="C58" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>327</v>
       </c>
@@ -2301,8 +3147,19 @@
       <c r="C59" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>328</v>
       </c>
@@ -2312,8 +3169,19 @@
       <c r="C60" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="1"/>
+        <v>350</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>329</v>
       </c>
@@ -2323,8 +3191,19 @@
       <c r="C61" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>330</v>
       </c>
@@ -2334,8 +3213,19 @@
       <c r="C62" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>331</v>
       </c>
@@ -2345,8 +3235,19 @@
       <c r="C63" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>332</v>
       </c>
@@ -2356,8 +3257,19 @@
       <c r="C64" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>333</v>
       </c>
@@ -2367,8 +3279,19 @@
       <c r="C65" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>334</v>
       </c>
@@ -2378,8 +3301,19 @@
       <c r="C66" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>335</v>
       </c>
@@ -2389,8 +3323,22 @@
       <c r="C67" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F130" si="2">3.14*0.025*0.025</f>
+        <v>1.9625000000000003E-3</v>
+      </c>
+      <c r="H67" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>336</v>
       </c>
@@ -2400,8 +3348,19 @@
       <c r="C68" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>50</v>
+      </c>
+      <c r="E68">
+        <f>50*63</f>
+        <v>3150</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>337</v>
       </c>
@@ -2411,8 +3370,19 @@
       <c r="C69" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>50</v>
+      </c>
+      <c r="E69">
+        <f>E68-50</f>
+        <v>3100</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>338</v>
       </c>
@@ -2422,8 +3392,19 @@
       <c r="C70" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>50</v>
+      </c>
+      <c r="E70">
+        <f>E69-50</f>
+        <v>3050</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>339</v>
       </c>
@@ -2433,8 +3414,19 @@
       <c r="C71" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>50</v>
+      </c>
+      <c r="E71">
+        <f t="shared" ref="E71:E131" si="3">E70-50</f>
+        <v>3000</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>340</v>
       </c>
@@ -2444,8 +3436,19 @@
       <c r="C72" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>50</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="3"/>
+        <v>2950</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>341</v>
       </c>
@@ -2455,8 +3458,19 @@
       <c r="C73" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>50</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="3"/>
+        <v>2900</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>342</v>
       </c>
@@ -2466,8 +3480,19 @@
       <c r="C74" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>50</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="3"/>
+        <v>2850</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>343</v>
       </c>
@@ -2477,8 +3502,19 @@
       <c r="C75" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>50</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="3"/>
+        <v>2800</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>344</v>
       </c>
@@ -2488,8 +3524,19 @@
       <c r="C76" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>50</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="3"/>
+        <v>2750</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>345</v>
       </c>
@@ -2499,8 +3546,19 @@
       <c r="C77" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>50</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="3"/>
+        <v>2700</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>346</v>
       </c>
@@ -2510,8 +3568,19 @@
       <c r="C78" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>50</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="3"/>
+        <v>2650</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>347</v>
       </c>
@@ -2521,8 +3590,19 @@
       <c r="C79" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>50</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="3"/>
+        <v>2600</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>348</v>
       </c>
@@ -2532,8 +3612,19 @@
       <c r="C80" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>50</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="3"/>
+        <v>2550</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>349</v>
       </c>
@@ -2543,8 +3634,19 @@
       <c r="C81" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>50</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="3"/>
+        <v>2500</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>350</v>
       </c>
@@ -2554,8 +3656,19 @@
       <c r="C82" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>50</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="3"/>
+        <v>2450</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>351</v>
       </c>
@@ -2565,8 +3678,19 @@
       <c r="C83" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>50</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="3"/>
+        <v>2400</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>352</v>
       </c>
@@ -2576,8 +3700,19 @@
       <c r="C84" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>50</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="3"/>
+        <v>2350</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>353</v>
       </c>
@@ -2587,8 +3722,19 @@
       <c r="C85" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>50</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="3"/>
+        <v>2300</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>354</v>
       </c>
@@ -2598,8 +3744,19 @@
       <c r="C86" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>50</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="3"/>
+        <v>2250</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>355</v>
       </c>
@@ -2609,8 +3766,19 @@
       <c r="C87" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>50</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="3"/>
+        <v>2200</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>356</v>
       </c>
@@ -2620,8 +3788,19 @@
       <c r="C88" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>50</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="3"/>
+        <v>2150</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>357</v>
       </c>
@@ -2631,8 +3810,19 @@
       <c r="C89" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>50</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="3"/>
+        <v>2100</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>358</v>
       </c>
@@ -2642,8 +3832,19 @@
       <c r="C90" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>50</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="3"/>
+        <v>2050</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>359</v>
       </c>
@@ -2653,8 +3854,19 @@
       <c r="C91" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>50</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="3"/>
+        <v>2000</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>360</v>
       </c>
@@ -2664,8 +3876,19 @@
       <c r="C92" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>50</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="3"/>
+        <v>1950</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>361</v>
       </c>
@@ -2675,8 +3898,19 @@
       <c r="C93" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>50</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="3"/>
+        <v>1900</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>362</v>
       </c>
@@ -2686,8 +3920,19 @@
       <c r="C94" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>50</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="3"/>
+        <v>1850</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>363</v>
       </c>
@@ -2697,8 +3942,19 @@
       <c r="C95" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>50</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="3"/>
+        <v>1800</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>364</v>
       </c>
@@ -2708,8 +3964,19 @@
       <c r="C96" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>50</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="3"/>
+        <v>1750</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>365</v>
       </c>
@@ -2719,8 +3986,19 @@
       <c r="C97" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>50</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="3"/>
+        <v>1700</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>366</v>
       </c>
@@ -2730,8 +4008,19 @@
       <c r="C98" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>50</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="3"/>
+        <v>1650</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>367</v>
       </c>
@@ -2741,8 +4030,19 @@
       <c r="C99" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>50</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="3"/>
+        <v>1600</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>368</v>
       </c>
@@ -2752,8 +4052,19 @@
       <c r="C100" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>50</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="3"/>
+        <v>1550</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>369</v>
       </c>
@@ -2763,8 +4074,19 @@
       <c r="C101" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>50</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="3"/>
+        <v>1500</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>370</v>
       </c>
@@ -2774,8 +4096,19 @@
       <c r="C102" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>50</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="3"/>
+        <v>1450</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>371</v>
       </c>
@@ -2785,8 +4118,19 @@
       <c r="C103" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>50</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="3"/>
+        <v>1400</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>372</v>
       </c>
@@ -2796,8 +4140,19 @@
       <c r="C104" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <v>50</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="3"/>
+        <v>1350</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>373</v>
       </c>
@@ -2807,8 +4162,19 @@
       <c r="C105" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <v>50</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="3"/>
+        <v>1300</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>374</v>
       </c>
@@ -2818,8 +4184,19 @@
       <c r="C106" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <v>50</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="3"/>
+        <v>1250</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>375</v>
       </c>
@@ -2829,8 +4206,19 @@
       <c r="C107" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <v>50</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="3"/>
+        <v>1200</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>376</v>
       </c>
@@ -2840,8 +4228,19 @@
       <c r="C108" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <v>50</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="3"/>
+        <v>1150</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>377</v>
       </c>
@@ -2851,8 +4250,19 @@
       <c r="C109" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <v>50</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="3"/>
+        <v>1100</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>378</v>
       </c>
@@ -2862,8 +4272,19 @@
       <c r="C110" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <v>50</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="3"/>
+        <v>1050</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>379</v>
       </c>
@@ -2873,8 +4294,19 @@
       <c r="C111" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <v>50</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>380</v>
       </c>
@@ -2884,8 +4316,19 @@
       <c r="C112" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <v>50</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="3"/>
+        <v>950</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>381</v>
       </c>
@@ -2895,8 +4338,19 @@
       <c r="C113" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <v>50</v>
+      </c>
+      <c r="E113">
+        <f t="shared" si="3"/>
+        <v>900</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>382</v>
       </c>
@@ -2906,8 +4360,19 @@
       <c r="C114" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <v>50</v>
+      </c>
+      <c r="E114">
+        <f t="shared" si="3"/>
+        <v>850</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>383</v>
       </c>
@@ -2917,8 +4382,19 @@
       <c r="C115" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <v>50</v>
+      </c>
+      <c r="E115">
+        <f t="shared" si="3"/>
+        <v>800</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>384</v>
       </c>
@@ -2928,8 +4404,19 @@
       <c r="C116" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <v>50</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="3"/>
+        <v>750</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>385</v>
       </c>
@@ -2939,8 +4426,19 @@
       <c r="C117" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <v>50</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="3"/>
+        <v>700</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>386</v>
       </c>
@@ -2950,8 +4448,19 @@
       <c r="C118" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118">
+        <v>50</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="3"/>
+        <v>650</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>387</v>
       </c>
@@ -2961,8 +4470,19 @@
       <c r="C119" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119">
+        <v>50</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="3"/>
+        <v>600</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>388</v>
       </c>
@@ -2972,8 +4492,19 @@
       <c r="C120" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120">
+        <v>50</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="3"/>
+        <v>550</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>389</v>
       </c>
@@ -2983,8 +4514,19 @@
       <c r="C121" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121">
+        <v>50</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>390</v>
       </c>
@@ -2994,8 +4536,19 @@
       <c r="C122" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122">
+        <v>50</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="3"/>
+        <v>450</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>391</v>
       </c>
@@ -3005,8 +4558,19 @@
       <c r="C123" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123">
+        <v>50</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="3"/>
+        <v>400</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>392</v>
       </c>
@@ -3016,8 +4580,19 @@
       <c r="C124" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124">
+        <v>50</v>
+      </c>
+      <c r="E124">
+        <f t="shared" si="3"/>
+        <v>350</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>393</v>
       </c>
@@ -3027,8 +4602,19 @@
       <c r="C125" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125">
+        <v>50</v>
+      </c>
+      <c r="E125">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>394</v>
       </c>
@@ -3038,8 +4624,19 @@
       <c r="C126" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126">
+        <v>50</v>
+      </c>
+      <c r="E126">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>395</v>
       </c>
@@ -3049,8 +4646,19 @@
       <c r="C127" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127">
+        <v>50</v>
+      </c>
+      <c r="E127">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>396</v>
       </c>
@@ -3060,8 +4668,19 @@
       <c r="C128" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D128">
+        <v>50</v>
+      </c>
+      <c r="E128">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>397</v>
       </c>
@@ -3071,8 +4690,19 @@
       <c r="C129" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D129">
+        <v>50</v>
+      </c>
+      <c r="E129">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>398</v>
       </c>
@@ -3082,8 +4712,19 @@
       <c r="C130" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <v>50</v>
+      </c>
+      <c r="E130">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="2"/>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>399</v>
       </c>
@@ -3093,26 +4734,37 @@
       <c r="C131" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D131">
+        <v>50</v>
+      </c>
+      <c r="E131">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <f t="shared" ref="F131" si="4">3.14*0.025*0.025</f>
+        <v>1.9625000000000003E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>156</v>
       </c>
       <c r="C132" t="s">
         <v>160</v>
       </c>
-      <c r="D132" t="s">
+      <c r="H132" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>157</v>
       </c>
       <c r="C133" t="s">
         <v>161</v>
       </c>
-      <c r="D133" t="s">
+      <c r="H133" t="s">
         <v>294</v>
       </c>
     </row>

</xml_diff>